<commit_message>
user page and superuser condition
</commit_message>
<xml_diff>
--- a/dashboard/media/exports/products.xlsx
+++ b/dashboard/media/exports/products.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,6 +1072,42 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>yes sir</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Don Valley</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>45401</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Anxiolytic</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Display total in overview page
</commit_message>
<xml_diff>
--- a/dashboard/media/exports/products.xlsx
+++ b/dashboard/media/exports/products.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -878,9 +878,6 @@
       <c r="E13" t="n">
         <v>80</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>45657</v>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>Antacids</t>
@@ -888,7 +885,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -924,7 +921,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -950,9 +947,6 @@
       <c r="E15" t="n">
         <v>140</v>
       </c>
-      <c r="F15" s="1" t="n">
-        <v>45657</v>
-      </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>Antacids</t>
@@ -960,7 +954,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -996,7 +990,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1026,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>
@@ -1068,43 +1062,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Tablet</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>yes sir</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Don Valley</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>12</v>
-      </c>
-      <c r="E19" t="n">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>45401</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Anxiolytic</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Tablet</t>
+          <t>Tablets</t>
         </is>
       </c>
     </row>

</xml_diff>